<commit_message>
category sale report 1
</commit_message>
<xml_diff>
--- a/temp/moin.xlsx
+++ b/temp/moin.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my django\mojallal24mehr\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mydjango\mojallal24mehr\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD5E4AD-3C83-4EDB-9C06-47B62918C595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CC24E0-692A-4598-8184-B5EDBFD81CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$102</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$111</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="109">
   <si>
     <t>kol</t>
   </si>
@@ -141,9 +141,6 @@
     <t>هزینه‌ هاي حقوق و دستمزد</t>
   </si>
   <si>
-    <t>ظرفشویی‌ دوو</t>
-  </si>
-  <si>
     <t>حساب اقساطی‌ مهر ایران</t>
   </si>
   <si>
@@ -262,6 +259,102 @@
   </si>
   <si>
     <t>حقوقي</t>
+  </si>
+  <si>
+    <t>كليه كالاها</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ريز آشپزخانه 2</t>
+  </si>
+  <si>
+    <t>يخچال و فريزر</t>
+  </si>
+  <si>
+    <t>لباسشويي</t>
+  </si>
+  <si>
+    <t>ظرفشويي</t>
+  </si>
+  <si>
+    <t>تلويزيون</t>
+  </si>
+  <si>
+    <t>اسپيکر</t>
+  </si>
+  <si>
+    <t>توکار ها / فر / هود / سينگ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">لوازم برقي ريز آشپزخانه </t>
+  </si>
+  <si>
+    <t>کولر آبي</t>
+  </si>
+  <si>
+    <t>کولر گازي</t>
+  </si>
+  <si>
+    <t>توستر / ماکروفر / فربرقي</t>
+  </si>
+  <si>
+    <t>جارو برقي / جارو شارژي</t>
+  </si>
+  <si>
+    <t>بخارشور</t>
+  </si>
+  <si>
+    <t>گرمايشي / بخاري</t>
+  </si>
+  <si>
+    <t>مبلمان / چوب / کالاي خواب</t>
+  </si>
+  <si>
+    <t xml:space="preserve">آرايشي بهداشتي </t>
+  </si>
+  <si>
+    <t xml:space="preserve">فرش / قاليچه </t>
+  </si>
+  <si>
+    <t>لوازم ريز آشپزخانه</t>
+  </si>
+  <si>
+    <t>حوله و روتختي</t>
+  </si>
+  <si>
+    <t>موبايل و لوازم جانبي</t>
+  </si>
+  <si>
+    <t xml:space="preserve">پلاستيک جات </t>
+  </si>
+  <si>
+    <t>لوازم خانگي دوو</t>
+  </si>
+  <si>
+    <t>قابلمه ها</t>
+  </si>
+  <si>
+    <t>فيک 1</t>
+  </si>
+  <si>
+    <t>فيک 2</t>
+  </si>
+  <si>
+    <t>فيک 3</t>
+  </si>
+  <si>
+    <t>فيک 4</t>
+  </si>
+  <si>
+    <t>فيک 5</t>
+  </si>
+  <si>
+    <t>فيک 6</t>
+  </si>
+  <si>
+    <t>فيک 7</t>
+  </si>
+  <si>
+    <t>فيک 8</t>
   </si>
 </sst>
 </file>
@@ -589,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:C109"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A88" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97:A100"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A30" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +724,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -642,7 +735,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -664,7 +757,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -672,10 +765,10 @@
         <v>102</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -683,10 +776,10 @@
         <v>102</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -694,10 +787,10 @@
         <v>102</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -705,10 +798,10 @@
         <v>102</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -716,10 +809,10 @@
         <v>102</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -727,10 +820,10 @@
         <v>102</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -738,10 +831,10 @@
         <v>102</v>
       </c>
       <c r="B13">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -749,10 +842,10 @@
         <v>102</v>
       </c>
       <c r="B14">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -760,10 +853,10 @@
         <v>102</v>
       </c>
       <c r="B15">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -771,10 +864,10 @@
         <v>102</v>
       </c>
       <c r="B16">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -782,10 +875,10 @@
         <v>102</v>
       </c>
       <c r="B17">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -793,10 +886,10 @@
         <v>102</v>
       </c>
       <c r="B18">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -804,10 +897,10 @@
         <v>102</v>
       </c>
       <c r="B19">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -815,10 +908,10 @@
         <v>102</v>
       </c>
       <c r="B20">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -826,10 +919,10 @@
         <v>102</v>
       </c>
       <c r="B21">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -837,10 +930,10 @@
         <v>102</v>
       </c>
       <c r="B22">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -848,10 +941,10 @@
         <v>102</v>
       </c>
       <c r="B23">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -859,10 +952,10 @@
         <v>102</v>
       </c>
       <c r="B24">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -870,10 +963,10 @@
         <v>102</v>
       </c>
       <c r="B25">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -881,10 +974,10 @@
         <v>102</v>
       </c>
       <c r="B26">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -892,10 +985,10 @@
         <v>102</v>
       </c>
       <c r="B27">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -903,10 +996,10 @@
         <v>102</v>
       </c>
       <c r="B28">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -914,10 +1007,10 @@
         <v>102</v>
       </c>
       <c r="B29">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C29" t="s">
-        <v>23</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -925,10 +1018,10 @@
         <v>102</v>
       </c>
       <c r="B30">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>37</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -936,109 +1029,109 @@
         <v>102</v>
       </c>
       <c r="B31">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C32" t="s">
-        <v>62</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C33" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="C34" t="s">
-        <v>51</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B35">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="C35" t="s">
-        <v>3</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B36">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="C36" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B37">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C37" t="s">
-        <v>65</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B38">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B39">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C39" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B40">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C40" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1046,10 +1139,10 @@
         <v>103</v>
       </c>
       <c r="B41">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1057,10 +1150,10 @@
         <v>103</v>
       </c>
       <c r="B42">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1068,10 +1161,10 @@
         <v>103</v>
       </c>
       <c r="B43">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1079,10 +1172,10 @@
         <v>103</v>
       </c>
       <c r="B44">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1090,10 +1183,10 @@
         <v>103</v>
       </c>
       <c r="B45">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1101,10 +1194,10 @@
         <v>103</v>
       </c>
       <c r="B46">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C46" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1112,10 +1205,10 @@
         <v>103</v>
       </c>
       <c r="B47">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C47" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1123,10 +1216,10 @@
         <v>103</v>
       </c>
       <c r="B48">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C48" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1134,10 +1227,10 @@
         <v>103</v>
       </c>
       <c r="B49">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C49" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1145,10 +1238,10 @@
         <v>103</v>
       </c>
       <c r="B50">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C50" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1156,10 +1249,10 @@
         <v>103</v>
       </c>
       <c r="B51">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C51" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1167,10 +1260,10 @@
         <v>103</v>
       </c>
       <c r="B52">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C52" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1178,230 +1271,230 @@
         <v>103</v>
       </c>
       <c r="B53">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C53" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B54">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C54" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C55" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>150</v>
+        <v>103</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C56" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>150</v>
+        <v>103</v>
       </c>
       <c r="B57">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C57" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>200</v>
+        <v>103</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C58" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>300</v>
+        <v>103</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C59" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>301</v>
+        <v>103</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C60" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>400</v>
+        <v>103</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C61" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>401</v>
+        <v>103</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C62" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>401</v>
+        <v>104</v>
       </c>
       <c r="B63">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>403</v>
+        <v>106</v>
       </c>
       <c r="B64">
         <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>500</v>
+        <v>150</v>
       </c>
       <c r="B65">
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>500</v>
+        <v>150</v>
       </c>
       <c r="B66">
         <v>2</v>
       </c>
       <c r="C66" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="B67">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="B68">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C68" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>500</v>
+        <v>301</v>
       </c>
       <c r="B69">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="B70">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>500</v>
+        <v>401</v>
       </c>
       <c r="B71">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C71" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>500</v>
+        <v>401</v>
       </c>
       <c r="B72">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C72" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>500</v>
+        <v>403</v>
       </c>
       <c r="B73">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1409,10 +1502,10 @@
         <v>500</v>
       </c>
       <c r="B74">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C74" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1420,10 +1513,10 @@
         <v>500</v>
       </c>
       <c r="B75">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C75" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1431,10 +1524,10 @@
         <v>500</v>
       </c>
       <c r="B76">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C76" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1442,10 +1535,10 @@
         <v>500</v>
       </c>
       <c r="B77">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C77" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -1453,10 +1546,10 @@
         <v>500</v>
       </c>
       <c r="B78">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C78" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -1464,10 +1557,10 @@
         <v>500</v>
       </c>
       <c r="B79">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C79" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -1475,10 +1568,10 @@
         <v>500</v>
       </c>
       <c r="B80">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C80" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -1486,10 +1579,10 @@
         <v>500</v>
       </c>
       <c r="B81">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C81" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -1497,10 +1590,10 @@
         <v>500</v>
       </c>
       <c r="B82">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C82" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -1508,10 +1601,10 @@
         <v>500</v>
       </c>
       <c r="B83">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C83" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -1519,10 +1612,10 @@
         <v>500</v>
       </c>
       <c r="B84">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C84" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -1530,10 +1623,10 @@
         <v>500</v>
       </c>
       <c r="B85">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C85" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -1541,10 +1634,10 @@
         <v>500</v>
       </c>
       <c r="B86">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C86" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -1552,10 +1645,10 @@
         <v>500</v>
       </c>
       <c r="B87">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C87" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -1563,148 +1656,247 @@
         <v>500</v>
       </c>
       <c r="B88">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C88" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B89">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C89" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B90">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C90" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B91">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C91" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B92">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C92" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="B93">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C93" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="B94">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C94" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>601</v>
+        <v>500</v>
       </c>
       <c r="B95">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C95" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
+        <v>500</v>
+      </c>
+      <c r="B96">
+        <v>26</v>
+      </c>
+      <c r="C96" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>500</v>
+      </c>
+      <c r="B97">
+        <v>28</v>
+      </c>
+      <c r="C97" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>501</v>
+      </c>
+      <c r="B98">
+        <v>1</v>
+      </c>
+      <c r="C98" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>501</v>
+      </c>
+      <c r="B99">
+        <v>2</v>
+      </c>
+      <c r="C99" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>501</v>
+      </c>
+      <c r="B100">
+        <v>3</v>
+      </c>
+      <c r="C100" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>501</v>
+      </c>
+      <c r="B101">
+        <v>4</v>
+      </c>
+      <c r="C101" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>600</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+      <c r="C102" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>600</v>
+      </c>
+      <c r="B103">
+        <v>2</v>
+      </c>
+      <c r="C103" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>601</v>
+      </c>
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="C104" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105">
         <v>602</v>
       </c>
-      <c r="B96">
+      <c r="B105">
         <v>1</v>
       </c>
-      <c r="C96" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <v>103</v>
-      </c>
-      <c r="B97">
+      <c r="C105" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>103</v>
+      </c>
+      <c r="B106">
         <v>27</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C106" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>103</v>
+      </c>
+      <c r="B107">
+        <v>28</v>
+      </c>
+      <c r="C107" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>103</v>
-      </c>
-      <c r="B98">
-        <v>28</v>
-      </c>
-      <c r="C98" s="1" t="s">
+    <row r="108" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>103</v>
+      </c>
+      <c r="B108">
+        <v>29</v>
+      </c>
+      <c r="C108" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A99">
-        <v>103</v>
-      </c>
-      <c r="B99">
-        <v>29</v>
-      </c>
-      <c r="C99" s="2" t="s">
+    <row r="109" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>103</v>
+      </c>
+      <c r="B109">
+        <v>30</v>
+      </c>
+      <c r="C109" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A100">
-        <v>103</v>
-      </c>
-      <c r="B100">
-        <v>30</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:C102" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C102">
-      <sortCondition ref="A1:A102"/>
+  <autoFilter ref="A1:C111" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C111">
+      <sortCondition ref="A1:A111"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>